<commit_message>
Adding the Mexico policy history to Vida
</commit_message>
<xml_diff>
--- a/Data/Querétaro/Misc/PolicyHistory.xlsx
+++ b/Data/Querétaro/Misc/PolicyHistory.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t xml:space="preserve">Data from</t>
   </si>
@@ -179,6 +179,36 @@
   </si>
   <si>
     <t xml:space="preserve">Acuerdo por el que se establecen las medidas sanitarias permanentes para la realización de las actividades económicas, productivas y sociales en el Estado de Querétaro, durante la emergencia sanitaria de la enfermedad COVID-19.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/Sep/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queretaro enters Scenario C: Containment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://noticiasdequeretaro.com.mx/2020/11/28/nuevo-sistema-de-indicadores-covid-19/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/Nov/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queretaro enters Scenario B: Prevention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://codiceinformativo.com/2020/11/que-pasaria-si-no-bajan-los-contagios-escenario-c-contempla-medidas-mas-restrictivas/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/Dec/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queretaro re-enters Scenario C: Containment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/Feb/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queretaro re-enters Scenario B: Prevention</t>
   </si>
 </sst>
 </file>
@@ -188,11 +218,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -208,6 +239,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -252,7 +297,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,8 +306,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -285,10 +342,10 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.43"/>
@@ -361,21 +418,21 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -384,12 +441,12 @@
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -398,12 +455,12 @@
       <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -412,7 +469,7 @@
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -420,10 +477,10 @@
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -454,7 +511,7 @@
       <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -472,17 +529,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -515,19 +572,43 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1"/>
+      <c r="A20" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1"/>
+      <c r="A21" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,6 +704,10 @@
       <c r="C44" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C18" r:id="rId1" display="https://noticiasdequeretaro.com.mx/2020/11/28/nuevo-sistema-de-indicadores-covid-19/"/>
+    <hyperlink ref="C19" r:id="rId2" display="https://codiceinformativo.com/2020/11/que-pasaria-si-no-bajan-los-contagios-escenario-c-contempla-medidas-mas-restrictivas/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>